<commit_message>
test: update template test
</commit_message>
<xml_diff>
--- a/tests/files/template.xlsx
+++ b/tests/files/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F87721-FFB8-4579-859F-B4013084CE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAD0F90-795A-4712-83AE-1EB93E209D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{6B887D9E-14EB-4971-A1EB-43D5D91379CE}"/>
+    <workbookView xWindow="-22545" yWindow="6045" windowWidth="22980" windowHeight="12090" xr2:uid="{6B887D9E-14EB-4971-A1EB-43D5D91379CE}"/>
   </bookViews>
   <sheets>
     <sheet name="tmp" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>titer[rowmeta]</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -55,6 +55,10 @@
   </si>
   <si>
     <t>[ignore]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ab[colmeta]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -504,14 +508,16 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -555,16 +561,36 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>